<commit_message>
update seagrass density spreadsheet
</commit_message>
<xml_diff>
--- a/spreadsheets_final/marinegeo_spreadsheet_seagrass_density.xlsx
+++ b/spreadsheets_final/marinegeo_spreadsheet_seagrass_density.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mlonn\Documents\Repositories\protocols\spreadsheets_final\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57E75542-BA1C-4CDF-BBD6-8DB62ADF81C5}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{585E0AC9-FFEA-4902-BE2C-A416A67E2E49}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="113">
   <si>
     <t>sheet</t>
   </si>
@@ -407,16 +407,10 @@
     </r>
   </si>
   <si>
-    <t>The method used to estimate cover: Braun-Blanquet, % bins, or point count.</t>
-  </si>
-  <si>
     <t xml:space="preserve">The total number of points counted in a quadrat to estimate cover. A value is only necessary if using the point count method, please leave this blank if using a different method. </t>
   </si>
   <si>
     <t>The date the sample was collected in the field (YYYY-MM-DD)</t>
-  </si>
-  <si>
-    <t>Cover code format will depend on the method used: Braun-Blanquet uses a letter scale (A, B, C, D, E) and % bins and point count methods use numeric scale. Refer to the protocol document for more information.</t>
   </si>
   <si>
     <t>The count of seagrass shoots within the quadrat. 
@@ -431,6 +425,18 @@
   </si>
   <si>
     <t>v0.5.0</t>
+  </si>
+  <si>
+    <t>quadrat_dimensions</t>
+  </si>
+  <si>
+    <t>Dimensions of the quadrat used during sampling (WxH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cover code format will depend on the method used: Braun-Blanquet uses a letter scale (A, B, C, D, E) and % bins and point count methods use numeric scale. Refer to the protocol document for more information. If reporting cover for substrate, leave scientific name blank for that row. </t>
+  </si>
+  <si>
+    <t>The method used to estimate cover: Braun-Blanquet, percent bins, or point count.</t>
   </si>
 </sst>
 </file>
@@ -1240,7 +1246,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="39.950000000000003" customHeight="1"/>
@@ -1309,7 +1315,7 @@
         <v>49</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="39.950000000000003" customHeight="1">
@@ -1376,11 +1382,11 @@
   <sheetPr>
     <tabColor rgb="FF97C8EB"/>
   </sheetPr>
-  <dimension ref="A1:N50"/>
+  <dimension ref="A1:O50"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -1393,12 +1399,12 @@
     <col min="7" max="7" width="30" style="1" customWidth="1"/>
     <col min="8" max="8" width="32.28515625" style="1" customWidth="1"/>
     <col min="9" max="9" width="19.140625" style="1" customWidth="1"/>
-    <col min="10" max="11" width="20.140625" style="1" customWidth="1"/>
-    <col min="12" max="13" width="21.42578125" customWidth="1"/>
-    <col min="14" max="14" width="25.5703125" customWidth="1"/>
+    <col min="10" max="12" width="20.140625" style="1" customWidth="1"/>
+    <col min="13" max="14" width="21.42578125" customWidth="1"/>
+    <col min="15" max="15" width="25.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="27" customFormat="1" ht="28.5" customHeight="1">
+    <row r="1" spans="1:15" s="27" customFormat="1" ht="28.5" customHeight="1">
       <c r="A1" s="25" t="s">
         <v>62</v>
       </c>
@@ -1430,363 +1436,366 @@
         <v>100</v>
       </c>
       <c r="K1" s="26" t="s">
+        <v>109</v>
+      </c>
+      <c r="L1" s="26" t="s">
         <v>101</v>
       </c>
-      <c r="L1" s="25" t="s">
+      <c r="M1" s="25" t="s">
         <v>98</v>
       </c>
-      <c r="M1" s="25" t="s">
+      <c r="N1" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="N1" s="25" t="s">
+      <c r="O1" s="25" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:15">
       <c r="A2" s="11"/>
       <c r="C2" s="2"/>
       <c r="D2" s="12"/>
-      <c r="L2" s="12"/>
       <c r="M2" s="12"/>
-    </row>
-    <row r="3" spans="1:14">
+      <c r="N2" s="12"/>
+    </row>
+    <row r="3" spans="1:15">
       <c r="A3" s="11"/>
       <c r="C3" s="2"/>
       <c r="D3" s="12"/>
-      <c r="L3" s="12"/>
       <c r="M3" s="12"/>
-    </row>
-    <row r="4" spans="1:14">
+      <c r="N3" s="12"/>
+    </row>
+    <row r="4" spans="1:15">
       <c r="A4" s="11"/>
       <c r="C4" s="2"/>
       <c r="D4" s="12"/>
-      <c r="L4" s="12"/>
       <c r="M4" s="12"/>
-    </row>
-    <row r="5" spans="1:14">
+      <c r="N4" s="12"/>
+    </row>
+    <row r="5" spans="1:15">
       <c r="A5" s="11"/>
       <c r="C5" s="2"/>
       <c r="D5" s="12"/>
-      <c r="L5" s="12"/>
       <c r="M5" s="12"/>
-    </row>
-    <row r="6" spans="1:14">
+      <c r="N5" s="12"/>
+    </row>
+    <row r="6" spans="1:15">
       <c r="A6" s="11"/>
       <c r="C6" s="2"/>
       <c r="D6" s="12"/>
-      <c r="L6" s="12"/>
       <c r="M6" s="12"/>
-    </row>
-    <row r="7" spans="1:14">
+      <c r="N6" s="12"/>
+    </row>
+    <row r="7" spans="1:15">
       <c r="A7" s="11"/>
       <c r="C7" s="2"/>
       <c r="D7" s="12"/>
-      <c r="L7" s="12"/>
       <c r="M7" s="12"/>
-    </row>
-    <row r="8" spans="1:14">
+      <c r="N7" s="12"/>
+    </row>
+    <row r="8" spans="1:15">
       <c r="A8" s="11"/>
       <c r="C8" s="2"/>
       <c r="D8" s="12"/>
-      <c r="L8" s="12"/>
       <c r="M8" s="12"/>
-    </row>
-    <row r="9" spans="1:14">
+      <c r="N8" s="12"/>
+    </row>
+    <row r="9" spans="1:15">
       <c r="A9" s="11"/>
       <c r="C9" s="2"/>
       <c r="D9" s="12"/>
-      <c r="L9" s="12"/>
       <c r="M9" s="12"/>
-    </row>
-    <row r="10" spans="1:14">
+      <c r="N9" s="12"/>
+    </row>
+    <row r="10" spans="1:15">
       <c r="A10" s="11"/>
       <c r="C10" s="2"/>
       <c r="D10" s="12"/>
-      <c r="L10" s="12"/>
       <c r="M10" s="12"/>
-    </row>
-    <row r="11" spans="1:14">
+      <c r="N10" s="12"/>
+    </row>
+    <row r="11" spans="1:15">
       <c r="A11" s="11"/>
       <c r="C11" s="2"/>
       <c r="D11" s="12"/>
-      <c r="L11" s="12"/>
       <c r="M11" s="12"/>
-    </row>
-    <row r="12" spans="1:14">
+      <c r="N11" s="12"/>
+    </row>
+    <row r="12" spans="1:15">
       <c r="A12" s="11"/>
       <c r="C12" s="2"/>
       <c r="D12" s="12"/>
-      <c r="L12" s="12"/>
       <c r="M12" s="12"/>
-    </row>
-    <row r="13" spans="1:14">
+      <c r="N12" s="12"/>
+    </row>
+    <row r="13" spans="1:15">
       <c r="A13" s="11"/>
       <c r="C13" s="2"/>
       <c r="D13" s="12"/>
-      <c r="L13" s="12"/>
       <c r="M13" s="12"/>
-    </row>
-    <row r="14" spans="1:14">
+      <c r="N13" s="12"/>
+    </row>
+    <row r="14" spans="1:15">
       <c r="A14" s="11"/>
       <c r="C14" s="2"/>
       <c r="D14" s="12"/>
-      <c r="L14" s="12"/>
       <c r="M14" s="12"/>
-    </row>
-    <row r="15" spans="1:14">
+      <c r="N14" s="12"/>
+    </row>
+    <row r="15" spans="1:15">
       <c r="A15" s="11"/>
       <c r="C15" s="2"/>
       <c r="D15" s="12"/>
-      <c r="L15" s="12"/>
       <c r="M15" s="12"/>
-    </row>
-    <row r="16" spans="1:14">
+      <c r="N15" s="12"/>
+    </row>
+    <row r="16" spans="1:15">
       <c r="A16" s="11"/>
       <c r="C16" s="2"/>
       <c r="D16" s="12"/>
-      <c r="L16" s="12"/>
       <c r="M16" s="12"/>
-    </row>
-    <row r="17" spans="1:13">
+      <c r="N16" s="12"/>
+    </row>
+    <row r="17" spans="1:14">
       <c r="A17" s="11"/>
       <c r="C17" s="2"/>
       <c r="D17" s="12"/>
-      <c r="L17" s="12"/>
       <c r="M17" s="12"/>
-    </row>
-    <row r="18" spans="1:13">
+      <c r="N17" s="12"/>
+    </row>
+    <row r="18" spans="1:14">
       <c r="A18" s="11"/>
       <c r="C18" s="2"/>
       <c r="D18" s="12"/>
-      <c r="L18" s="12"/>
       <c r="M18" s="12"/>
-    </row>
-    <row r="19" spans="1:13">
+      <c r="N18" s="12"/>
+    </row>
+    <row r="19" spans="1:14">
       <c r="A19" s="11"/>
       <c r="C19" s="2"/>
       <c r="D19" s="12"/>
-      <c r="L19" s="12"/>
       <c r="M19" s="12"/>
-    </row>
-    <row r="20" spans="1:13">
+      <c r="N19" s="12"/>
+    </row>
+    <row r="20" spans="1:14">
       <c r="A20" s="11"/>
       <c r="C20" s="2"/>
       <c r="D20" s="12"/>
-      <c r="L20" s="12"/>
       <c r="M20" s="12"/>
-    </row>
-    <row r="21" spans="1:13">
+      <c r="N20" s="12"/>
+    </row>
+    <row r="21" spans="1:14">
       <c r="A21" s="11"/>
       <c r="C21" s="2"/>
       <c r="D21" s="12"/>
-      <c r="L21" s="12"/>
       <c r="M21" s="12"/>
-    </row>
-    <row r="22" spans="1:13">
+      <c r="N21" s="12"/>
+    </row>
+    <row r="22" spans="1:14">
       <c r="A22" s="11"/>
       <c r="C22" s="2"/>
       <c r="D22" s="12"/>
-      <c r="L22" s="12"/>
       <c r="M22" s="12"/>
-    </row>
-    <row r="23" spans="1:13">
+      <c r="N22" s="12"/>
+    </row>
+    <row r="23" spans="1:14">
       <c r="A23" s="11"/>
       <c r="C23" s="2"/>
       <c r="D23" s="12"/>
-      <c r="L23" s="12"/>
       <c r="M23" s="12"/>
-    </row>
-    <row r="24" spans="1:13">
+      <c r="N23" s="12"/>
+    </row>
+    <row r="24" spans="1:14">
       <c r="A24" s="11"/>
       <c r="C24" s="2"/>
       <c r="D24" s="12"/>
-      <c r="L24" s="12"/>
       <c r="M24" s="12"/>
-    </row>
-    <row r="25" spans="1:13">
+      <c r="N24" s="12"/>
+    </row>
+    <row r="25" spans="1:14">
       <c r="A25" s="11"/>
       <c r="C25" s="2"/>
       <c r="D25" s="12"/>
-      <c r="L25" s="12"/>
       <c r="M25" s="12"/>
-    </row>
-    <row r="26" spans="1:13">
+      <c r="N25" s="12"/>
+    </row>
+    <row r="26" spans="1:14">
       <c r="A26" s="11"/>
       <c r="C26" s="2"/>
       <c r="D26" s="12"/>
-      <c r="L26" s="12"/>
       <c r="M26" s="12"/>
-    </row>
-    <row r="27" spans="1:13">
+      <c r="N26" s="12"/>
+    </row>
+    <row r="27" spans="1:14">
       <c r="A27" s="11"/>
       <c r="C27" s="2"/>
       <c r="D27" s="12"/>
-      <c r="L27" s="12"/>
       <c r="M27" s="12"/>
-    </row>
-    <row r="28" spans="1:13">
+      <c r="N27" s="12"/>
+    </row>
+    <row r="28" spans="1:14">
       <c r="A28" s="11"/>
       <c r="C28" s="2"/>
       <c r="D28" s="12"/>
-      <c r="L28" s="12"/>
       <c r="M28" s="12"/>
-    </row>
-    <row r="29" spans="1:13">
+      <c r="N28" s="12"/>
+    </row>
+    <row r="29" spans="1:14">
       <c r="A29" s="11"/>
       <c r="C29" s="2"/>
       <c r="D29" s="12"/>
-      <c r="L29" s="12"/>
       <c r="M29" s="12"/>
-    </row>
-    <row r="30" spans="1:13">
+      <c r="N29" s="12"/>
+    </row>
+    <row r="30" spans="1:14">
       <c r="A30" s="11"/>
       <c r="C30" s="2"/>
       <c r="D30" s="12"/>
-      <c r="L30" s="12"/>
       <c r="M30" s="12"/>
-    </row>
-    <row r="31" spans="1:13">
+      <c r="N30" s="12"/>
+    </row>
+    <row r="31" spans="1:14">
       <c r="A31" s="11"/>
       <c r="C31" s="2"/>
       <c r="D31" s="12"/>
-      <c r="L31" s="12"/>
       <c r="M31" s="12"/>
-    </row>
-    <row r="32" spans="1:13">
+      <c r="N31" s="12"/>
+    </row>
+    <row r="32" spans="1:14">
       <c r="A32" s="11"/>
       <c r="C32" s="2"/>
       <c r="D32" s="12"/>
-      <c r="L32" s="12"/>
       <c r="M32" s="12"/>
-    </row>
-    <row r="33" spans="1:13">
+      <c r="N32" s="12"/>
+    </row>
+    <row r="33" spans="1:14">
       <c r="A33" s="11"/>
       <c r="C33" s="2"/>
       <c r="D33" s="12"/>
-      <c r="L33" s="12"/>
       <c r="M33" s="12"/>
-    </row>
-    <row r="34" spans="1:13">
+      <c r="N33" s="12"/>
+    </row>
+    <row r="34" spans="1:14">
       <c r="A34" s="11"/>
       <c r="C34" s="2"/>
       <c r="D34" s="12"/>
-      <c r="L34" s="12"/>
       <c r="M34" s="12"/>
-    </row>
-    <row r="35" spans="1:13">
+      <c r="N34" s="12"/>
+    </row>
+    <row r="35" spans="1:14">
       <c r="A35" s="11"/>
       <c r="C35" s="2"/>
       <c r="D35" s="12"/>
-      <c r="L35" s="12"/>
       <c r="M35" s="12"/>
-    </row>
-    <row r="36" spans="1:13">
+      <c r="N35" s="12"/>
+    </row>
+    <row r="36" spans="1:14">
       <c r="A36" s="11"/>
       <c r="C36" s="2"/>
       <c r="D36" s="12"/>
-      <c r="L36" s="12"/>
       <c r="M36" s="12"/>
-    </row>
-    <row r="37" spans="1:13">
+      <c r="N36" s="12"/>
+    </row>
+    <row r="37" spans="1:14">
       <c r="A37" s="11"/>
       <c r="C37" s="2"/>
       <c r="D37" s="12"/>
-      <c r="L37" s="12"/>
       <c r="M37" s="12"/>
-    </row>
-    <row r="38" spans="1:13">
+      <c r="N37" s="12"/>
+    </row>
+    <row r="38" spans="1:14">
       <c r="A38" s="11"/>
       <c r="C38" s="2"/>
       <c r="D38" s="12"/>
-      <c r="L38" s="12"/>
       <c r="M38" s="12"/>
-    </row>
-    <row r="39" spans="1:13">
+      <c r="N38" s="12"/>
+    </row>
+    <row r="39" spans="1:14">
       <c r="A39" s="11"/>
       <c r="C39" s="2"/>
       <c r="D39" s="12"/>
-      <c r="L39" s="12"/>
       <c r="M39" s="12"/>
-    </row>
-    <row r="40" spans="1:13">
+      <c r="N39" s="12"/>
+    </row>
+    <row r="40" spans="1:14">
       <c r="A40" s="11"/>
       <c r="C40" s="2"/>
       <c r="D40" s="12"/>
-      <c r="L40" s="12"/>
       <c r="M40" s="12"/>
-    </row>
-    <row r="41" spans="1:13">
+      <c r="N40" s="12"/>
+    </row>
+    <row r="41" spans="1:14">
       <c r="A41" s="11"/>
       <c r="C41" s="2"/>
       <c r="D41" s="12"/>
-      <c r="L41" s="12"/>
       <c r="M41" s="12"/>
-    </row>
-    <row r="42" spans="1:13">
+      <c r="N41" s="12"/>
+    </row>
+    <row r="42" spans="1:14">
       <c r="A42" s="11"/>
       <c r="C42" s="2"/>
       <c r="D42" s="12"/>
-      <c r="L42" s="12"/>
       <c r="M42" s="12"/>
-    </row>
-    <row r="43" spans="1:13">
+      <c r="N42" s="12"/>
+    </row>
+    <row r="43" spans="1:14">
       <c r="A43" s="11"/>
       <c r="C43" s="2"/>
       <c r="D43" s="12"/>
-      <c r="L43" s="12"/>
       <c r="M43" s="12"/>
-    </row>
-    <row r="44" spans="1:13">
+      <c r="N43" s="12"/>
+    </row>
+    <row r="44" spans="1:14">
       <c r="A44" s="11"/>
       <c r="C44" s="2"/>
       <c r="D44" s="12"/>
-      <c r="L44" s="12"/>
       <c r="M44" s="12"/>
-    </row>
-    <row r="45" spans="1:13">
+      <c r="N44" s="12"/>
+    </row>
+    <row r="45" spans="1:14">
       <c r="A45" s="11"/>
       <c r="C45" s="2"/>
       <c r="D45" s="12"/>
-      <c r="L45" s="12"/>
       <c r="M45" s="12"/>
-    </row>
-    <row r="46" spans="1:13">
+      <c r="N45" s="12"/>
+    </row>
+    <row r="46" spans="1:14">
       <c r="A46" s="11"/>
       <c r="C46" s="2"/>
       <c r="D46" s="12"/>
-      <c r="L46" s="12"/>
       <c r="M46" s="12"/>
-    </row>
-    <row r="47" spans="1:13">
+      <c r="N46" s="12"/>
+    </row>
+    <row r="47" spans="1:14">
       <c r="A47" s="11"/>
       <c r="C47" s="2"/>
       <c r="D47" s="12"/>
-      <c r="L47" s="12"/>
       <c r="M47" s="12"/>
-    </row>
-    <row r="48" spans="1:13">
+      <c r="N47" s="12"/>
+    </row>
+    <row r="48" spans="1:14">
       <c r="A48" s="11"/>
       <c r="C48" s="2"/>
       <c r="D48" s="12"/>
-      <c r="L48" s="12"/>
       <c r="M48" s="12"/>
-    </row>
-    <row r="49" spans="1:13">
+      <c r="N48" s="12"/>
+    </row>
+    <row r="49" spans="1:14">
       <c r="A49" s="11"/>
       <c r="C49" s="2"/>
       <c r="D49" s="12"/>
-      <c r="L49" s="12"/>
       <c r="M49" s="12"/>
-    </row>
-    <row r="50" spans="1:13">
+      <c r="N49" s="12"/>
+    </row>
+    <row r="50" spans="1:14">
       <c r="A50" s="11"/>
       <c r="C50" s="2"/>
       <c r="D50" s="12"/>
-      <c r="L50" s="12"/>
       <c r="M50" s="12"/>
+      <c r="N50" s="12"/>
     </row>
   </sheetData>
-  <dataValidations count="13">
+  <dataValidations count="14">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter your 6 character code (XXX-YYY). _x000a__x000a_Codes can be found in the standards section of the MarineGEO protocol website @ https://marinegeo.github.io/standards/" sqref="B1" xr:uid="{00000000-0002-0000-0100-000000000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The name of the specific location where the sample was collected; e.g., Curlew Cay" sqref="C1" xr:uid="{00000000-0002-0000-0100-000001000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The date the sample was collected in the field (YYYY-MM-DD)" sqref="A1" xr:uid="{00000000-0002-0000-0100-000002000000}"/>
@@ -1794,12 +1803,13 @@
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Longitude in decimal degrees to five decimal places" sqref="F1 H1" xr:uid="{00000000-0002-0000-0100-000004000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Site depth in meters. _x000a__x000a_For sites spanning a depth range, please provide a single, average depth." sqref="I1" xr:uid="{00000000-0002-0000-0100-000005000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The transect at the location the sample came from: 1, 2, or 3" sqref="D1" xr:uid="{00000000-0002-0000-0100-000007000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Name(s) of data collector(s)" sqref="L1" xr:uid="{44C8B047-51F0-4042-A1C0-BC63B61AA2BD}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Any additional notes regarding observations, context, or concerns about the data." sqref="N1" xr:uid="{273894AA-C7F6-494C-90C2-0426038084EA}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Full name of the data entry person" sqref="M1" xr:uid="{74D42E31-A654-4C44-8B91-B625C81C4548}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The total number of points counted in a quadrat to estimate cover. A value is only necessary if using the point count method, please leave this blank if using a different method. " sqref="K1" xr:uid="{00000000-0002-0000-0200-000000000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Note the type of bare substratum (ex. sand, mud, mixed)" sqref="K1" xr:uid="{1CC2CF78-5CA6-CB45-96E3-90627B27E7F6}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The method used to estimate cover: Braun-Blanquet, % bins, or point count." sqref="J1 J1" xr:uid="{4D844A01-CCE5-42A5-9755-35D9B85263BB}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Name(s) of data collector(s)" sqref="M1" xr:uid="{44C8B047-51F0-4042-A1C0-BC63B61AA2BD}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Any additional notes regarding observations, context, or concerns about the data." sqref="O1" xr:uid="{273894AA-C7F6-494C-90C2-0426038084EA}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Full name of the data entry person" sqref="N1" xr:uid="{74D42E31-A654-4C44-8B91-B625C81C4548}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The total number of points counted in a quadrat to estimate cover. A value is only necessary if using the point count method, please leave this blank if using a different method. " sqref="L1" xr:uid="{00000000-0002-0000-0200-000000000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Note the type of bare substratum (ex. sand, mud, mixed)" sqref="L1" xr:uid="{1CC2CF78-5CA6-CB45-96E3-90627B27E7F6}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Dimensions of the quadrat used during sampling (WxH)" sqref="K1" xr:uid="{41F2C8E9-58C2-493E-9BC8-ED15E2709EB5}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The method used to estimate cover: Braun-Blanquet, percent_x000a_ bins, or point count." sqref="J1" xr:uid="{5010063D-5B2E-4F18-9FA0-0CDEF088106B}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1814,7 +1824,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -2107,12 +2117,12 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
   <dataValidations count="9">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Cover code format will depend on the method used: Braun-Blanquet uses a letter scale (A, B, C, D, E) and % bins and point count methods use numeric scale. Refer to the protocol document for more information." sqref="H1" xr:uid="{00000000-0002-0000-0200-000002000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Cover code format will depend on the method used: Braun-Blanquet uses a letter scale (A, B, C, D, E) and % bins and point count methods use numeric scale. Refer to the protocol document for more information." sqref="H1:I1" xr:uid="{00000000-0002-0000-0200-000002000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The transect at the location the sample came from: 1, 2, or 3" sqref="D1" xr:uid="{00000000-0002-0000-0200-000003000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The date the sample was collected in the field (YYYY-MM-DD)" sqref="A1" xr:uid="{00000000-0002-0000-0200-000004000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The name of the specific location where the sample was collected; e.g., Curlew Cay" sqref="C1" xr:uid="{00000000-0002-0000-0200-000005000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter your 6 character code (XXX-YYY). _x000a__x000a_Codes can be found in the standards section of the MarineGEO protocol website @ https://marinegeo.github.io/standards/" sqref="B1" xr:uid="{00000000-0002-0000-0200-000006000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Any additional notes regarding observations, context, or concerns about the data." sqref="J1 G1" xr:uid="{8CFD2252-77F3-784F-BE9B-CFBFF8E3C6D9}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Any additional notes regarding observations, context, or concerns about the data." sqref="I1:J1 G1" xr:uid="{8CFD2252-77F3-784F-BE9B-CFBFF8E3C6D9}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Scientific name using standard scientific nomenclature. If the species cannot be identified to species, report genus or higher." sqref="F1" xr:uid="{8B323C89-0455-7E49-B6A4-C3889CE1B426}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The distance along the transect that the sample was collected (from 1-50 m)" sqref="E1" xr:uid="{00000000-0002-0000-0200-000000000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Note the type of bare substratum (ex. sand, mud, mixed)" sqref="I1" xr:uid="{1CC2CF78-5CA6-CB45-96E3-90627B27E7F6}"/>
@@ -2761,11 +2771,11 @@
   <sheetPr>
     <tabColor rgb="FF97C8EB"/>
   </sheetPr>
-  <dimension ref="A1:F67"/>
+  <dimension ref="A1:F68"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="60" customHeight="1"/>
@@ -3000,7 +3010,7 @@
         <v>62</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D14" s="6" t="s">
         <v>2</v>
@@ -3150,7 +3160,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:6" s="23" customFormat="1" ht="31.5">
+    <row r="23" spans="1:6" s="23" customFormat="1" ht="47.25">
       <c r="A23" s="6" t="s">
         <v>58</v>
       </c>
@@ -3158,7 +3168,7 @@
         <v>100</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>103</v>
+        <v>112</v>
       </c>
       <c r="D23" s="6" t="s">
         <v>14</v>
@@ -3166,34 +3176,34 @@
       <c r="E23" s="6"/>
       <c r="F23" s="6"/>
     </row>
-    <row r="24" spans="1:6" s="23" customFormat="1" ht="78.75">
+    <row r="24" spans="1:6" s="23" customFormat="1" ht="31.5">
       <c r="A24" s="6" t="s">
         <v>58</v>
       </c>
       <c r="B24" s="32" t="s">
-        <v>101</v>
+        <v>109</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="E24" s="6"/>
       <c r="F24" s="6"/>
     </row>
-    <row r="25" spans="1:6" s="37" customFormat="1" ht="60" customHeight="1">
+    <row r="25" spans="1:6" s="23" customFormat="1" ht="78.75">
       <c r="A25" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="B25" s="36" t="s">
-        <v>98</v>
+      <c r="B25" s="32" t="s">
+        <v>101</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>94</v>
+        <v>103</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="E25" s="6"/>
       <c r="F25" s="6"/>
@@ -3203,10 +3213,10 @@
         <v>58</v>
       </c>
       <c r="B26" s="36" t="s">
-        <v>46</v>
+        <v>98</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="D26" s="6" t="s">
         <v>14</v>
@@ -3214,15 +3224,15 @@
       <c r="E26" s="6"/>
       <c r="F26" s="6"/>
     </row>
-    <row r="27" spans="1:6" s="23" customFormat="1" ht="47.25">
+    <row r="27" spans="1:6" s="37" customFormat="1" ht="60" customHeight="1">
       <c r="A27" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="B27" s="6" t="s">
-        <v>86</v>
+      <c r="B27" s="36" t="s">
+        <v>46</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="D27" s="6" t="s">
         <v>14</v>
@@ -3230,129 +3240,129 @@
       <c r="E27" s="6"/>
       <c r="F27" s="6"/>
     </row>
-    <row r="28" spans="1:6" s="23" customFormat="1" ht="31.5">
-      <c r="A28" s="13" t="s">
+    <row r="28" spans="1:6" s="23" customFormat="1" ht="47.25">
+      <c r="A28" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E28" s="6"/>
+      <c r="F28" s="6"/>
+    </row>
+    <row r="29" spans="1:6" s="23" customFormat="1" ht="31.5">
+      <c r="A29" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="B28" s="13"/>
-      <c r="C28" s="13" t="s">
+      <c r="B29" s="13"/>
+      <c r="C29" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="D28" s="13"/>
-      <c r="E28" s="13"/>
-      <c r="F28" s="13"/>
-    </row>
-    <row r="29" spans="1:6" s="23" customFormat="1" ht="31.5">
-      <c r="A29" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="B29" s="31" t="s">
-        <v>62</v>
-      </c>
-      <c r="C29" s="31" t="s">
-        <v>105</v>
-      </c>
-      <c r="D29" s="31" t="s">
-        <v>2</v>
-      </c>
-      <c r="E29" s="31" t="s">
-        <v>3</v>
-      </c>
-      <c r="F29" s="31"/>
-    </row>
-    <row r="30" spans="1:6" s="23" customFormat="1" ht="72.75" customHeight="1">
+      <c r="D29" s="13"/>
+      <c r="E29" s="13"/>
+      <c r="F29" s="13"/>
+    </row>
+    <row r="30" spans="1:6" s="23" customFormat="1" ht="31.5">
       <c r="A30" s="10" t="s">
         <v>59</v>
       </c>
       <c r="B30" s="31" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="C30" s="31" t="s">
-        <v>25</v>
+        <v>104</v>
       </c>
       <c r="D30" s="31" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="E30" s="31" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F30" s="31"/>
     </row>
-    <row r="31" spans="1:6" s="23" customFormat="1" ht="47.25">
+    <row r="31" spans="1:6" s="23" customFormat="1" ht="72.75" customHeight="1">
       <c r="A31" s="10" t="s">
         <v>59</v>
       </c>
       <c r="B31" s="31" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="C31" s="31" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="D31" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="E31" s="31"/>
+      <c r="E31" s="31" t="s">
+        <v>6</v>
+      </c>
       <c r="F31" s="31"/>
     </row>
-    <row r="32" spans="1:6" s="18" customFormat="1" ht="60" customHeight="1">
+    <row r="32" spans="1:6" s="23" customFormat="1" ht="47.25">
       <c r="A32" s="10" t="s">
         <v>59</v>
       </c>
       <c r="B32" s="31" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C32" s="31" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="D32" s="31" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="E32" s="31"/>
       <c r="F32" s="31"/>
     </row>
-    <row r="33" spans="1:6" s="19" customFormat="1" ht="31.5">
+    <row r="33" spans="1:6" s="18" customFormat="1" ht="60" customHeight="1">
       <c r="A33" s="10" t="s">
         <v>59</v>
       </c>
       <c r="B33" s="31" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="C33" s="31" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="D33" s="31" t="s">
         <v>27</v>
       </c>
       <c r="E33" s="31"/>
-      <c r="F33" s="31" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" s="30" customFormat="1" ht="66" customHeight="1">
+      <c r="F33" s="31"/>
+    </row>
+    <row r="34" spans="1:6" s="19" customFormat="1" ht="31.5">
       <c r="A34" s="10" t="s">
         <v>59</v>
       </c>
       <c r="B34" s="31" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="C34" s="31" t="s">
-        <v>97</v>
+        <v>28</v>
       </c>
       <c r="D34" s="31" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="E34" s="31"/>
-      <c r="F34" s="31"/>
+      <c r="F34" s="31" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="35" spans="1:6" s="30" customFormat="1" ht="66" customHeight="1">
       <c r="A35" s="10" t="s">
         <v>59</v>
       </c>
       <c r="B35" s="31" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C35" s="31" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="D35" s="31" t="s">
         <v>14</v>
@@ -3360,45 +3370,45 @@
       <c r="E35" s="31"/>
       <c r="F35" s="31"/>
     </row>
-    <row r="36" spans="1:6" s="19" customFormat="1" ht="94.5">
+    <row r="36" spans="1:6" s="30" customFormat="1" ht="66" customHeight="1">
       <c r="A36" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="B36" s="33" t="s">
-        <v>70</v>
+      <c r="B36" s="31" t="s">
+        <v>96</v>
       </c>
       <c r="C36" s="31" t="s">
-        <v>106</v>
-      </c>
-      <c r="D36" s="31"/>
+        <v>90</v>
+      </c>
+      <c r="D36" s="31" t="s">
+        <v>14</v>
+      </c>
       <c r="E36" s="31"/>
       <c r="F36" s="31"/>
     </row>
-    <row r="37" spans="1:6" s="19" customFormat="1" ht="31.5">
+    <row r="37" spans="1:6" s="19" customFormat="1" ht="127.5" customHeight="1">
       <c r="A37" s="10" t="s">
         <v>59</v>
       </c>
       <c r="B37" s="33" t="s">
-        <v>92</v>
+        <v>70</v>
       </c>
       <c r="C37" s="31" t="s">
-        <v>93</v>
-      </c>
-      <c r="D37" s="31" t="s">
-        <v>14</v>
-      </c>
+        <v>111</v>
+      </c>
+      <c r="D37" s="31"/>
       <c r="E37" s="31"/>
       <c r="F37" s="31"/>
     </row>
-    <row r="38" spans="1:6" s="19" customFormat="1" ht="49.5" customHeight="1">
+    <row r="38" spans="1:6" s="19" customFormat="1" ht="31.5">
       <c r="A38" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="B38" s="10" t="s">
-        <v>87</v>
+      <c r="B38" s="33" t="s">
+        <v>92</v>
       </c>
       <c r="C38" s="31" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="D38" s="31" t="s">
         <v>14</v>
@@ -3406,129 +3416,129 @@
       <c r="E38" s="31"/>
       <c r="F38" s="31"/>
     </row>
-    <row r="39" spans="1:6" s="19" customFormat="1" ht="31.5">
-      <c r="A39" s="13" t="s">
-        <v>109</v>
-      </c>
-      <c r="B39" s="14"/>
-      <c r="C39" s="13" t="s">
+    <row r="39" spans="1:6" s="19" customFormat="1" ht="49.5" customHeight="1">
+      <c r="A39" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="B39" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="C39" s="31" t="s">
+        <v>90</v>
+      </c>
+      <c r="D39" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="E39" s="31"/>
+      <c r="F39" s="31"/>
+    </row>
+    <row r="40" spans="1:6" s="19" customFormat="1" ht="31.5">
+      <c r="A40" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="B40" s="14"/>
+      <c r="C40" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="D39" s="14"/>
-      <c r="E39" s="14"/>
-      <c r="F39" s="14"/>
-    </row>
-    <row r="40" spans="1:6" s="19" customFormat="1" ht="39.75" customHeight="1">
-      <c r="A40" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="B40" s="22" t="s">
+      <c r="D40" s="14"/>
+      <c r="E40" s="14"/>
+      <c r="F40" s="14"/>
+    </row>
+    <row r="41" spans="1:6" s="19" customFormat="1" ht="39.75" customHeight="1">
+      <c r="A41" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="B41" s="22" t="s">
         <v>62</v>
       </c>
-      <c r="C40" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="D40" s="5" t="s">
+      <c r="C41" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="D41" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E40" s="5" t="s">
+      <c r="E41" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="F40" s="5"/>
-    </row>
-    <row r="41" spans="1:6" s="19" customFormat="1" ht="71.25" customHeight="1">
-      <c r="A41" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="B41" s="22" t="s">
+      <c r="F41" s="5"/>
+    </row>
+    <row r="42" spans="1:6" s="19" customFormat="1" ht="71.25" customHeight="1">
+      <c r="A42" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="B42" s="22" t="s">
         <v>75</v>
       </c>
-      <c r="C41" s="5" t="s">
+      <c r="C42" s="5" t="s">
         <v>25</v>
-      </c>
-      <c r="D41" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E41" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="F41" s="5"/>
-    </row>
-    <row r="42" spans="1:6" s="18" customFormat="1" ht="35.25" customHeight="1">
-      <c r="A42" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="B42" s="22" t="s">
-        <v>61</v>
-      </c>
-      <c r="C42" s="5" t="s">
-        <v>7</v>
       </c>
       <c r="D42" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E42" s="5"/>
+      <c r="E42" s="5" t="s">
+        <v>6</v>
+      </c>
       <c r="F42" s="5"/>
     </row>
-    <row r="43" spans="1:6" s="19" customFormat="1" ht="42" customHeight="1">
+    <row r="43" spans="1:6" s="18" customFormat="1" ht="35.25" customHeight="1">
       <c r="A43" s="5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B43" s="22" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="E43" s="5"/>
       <c r="F43" s="5"/>
     </row>
-    <row r="44" spans="1:6" s="19" customFormat="1" ht="39" customHeight="1">
+    <row r="44" spans="1:6" s="19" customFormat="1" ht="42" customHeight="1">
       <c r="A44" s="5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B44" s="22" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="D44" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="E44" s="22"/>
-      <c r="F44" s="5" t="s">
+      <c r="E44" s="5"/>
+      <c r="F44" s="5"/>
+    </row>
+    <row r="45" spans="1:6" s="19" customFormat="1" ht="39" customHeight="1">
+      <c r="A45" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="B45" s="22" t="s">
+        <v>69</v>
+      </c>
+      <c r="C45" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D45" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E45" s="22"/>
+      <c r="F45" s="5" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" s="30" customFormat="1" ht="66" customHeight="1">
-      <c r="A45" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="B45" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="C45" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="D45" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E45" s="5"/>
-      <c r="F45" s="5"/>
     </row>
     <row r="46" spans="1:6" s="30" customFormat="1" ht="66" customHeight="1">
       <c r="A46" s="5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="D46" s="5" t="s">
         <v>14</v>
@@ -3536,165 +3546,165 @@
       <c r="E46" s="5"/>
       <c r="F46" s="5"/>
     </row>
-    <row r="47" spans="1:6" s="19" customFormat="1" ht="78.75">
+    <row r="47" spans="1:6" s="30" customFormat="1" ht="66" customHeight="1">
       <c r="A47" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="B47" s="22" t="s">
+        <v>107</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="C47" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="D47" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E47" s="5"/>
+      <c r="F47" s="5"/>
+    </row>
+    <row r="48" spans="1:6" s="19" customFormat="1" ht="78.75">
+      <c r="A48" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="B48" s="22" t="s">
         <v>74</v>
       </c>
-      <c r="C47" s="5" t="s">
+      <c r="C48" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="D47" s="5" t="s">
+      <c r="D48" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="E47" s="22" t="s">
+      <c r="E48" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="F47" s="5" t="s">
+      <c r="F48" s="5" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="48" spans="1:6" s="19" customFormat="1" ht="55.5" customHeight="1">
-      <c r="A48" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="B48" s="5" t="s">
+    <row r="49" spans="1:6" s="19" customFormat="1" ht="55.5" customHeight="1">
+      <c r="A49" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="B49" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="C48" s="5" t="s">
+      <c r="C49" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="D48" s="5" t="s">
+      <c r="D49" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E48" s="22"/>
-      <c r="F48" s="5"/>
-    </row>
-    <row r="49" spans="1:6" s="19" customFormat="1" ht="47.25">
-      <c r="A49" s="13" t="s">
+      <c r="E49" s="22"/>
+      <c r="F49" s="5"/>
+    </row>
+    <row r="50" spans="1:6" s="19" customFormat="1" ht="47.25">
+      <c r="A50" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="B49" s="13"/>
-      <c r="C49" s="13" t="s">
+      <c r="B50" s="13"/>
+      <c r="C50" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="D49" s="13"/>
-      <c r="E49" s="14"/>
-      <c r="F49" s="13"/>
-    </row>
-    <row r="50" spans="1:6" s="15" customFormat="1" ht="60" customHeight="1">
-      <c r="A50" s="31" t="s">
-        <v>91</v>
-      </c>
-      <c r="B50" s="34" t="s">
-        <v>62</v>
-      </c>
-      <c r="C50" s="31" t="s">
-        <v>105</v>
-      </c>
-      <c r="D50" s="31" t="s">
-        <v>2</v>
-      </c>
-      <c r="E50" s="31" t="s">
-        <v>3</v>
-      </c>
-      <c r="F50" s="31"/>
-    </row>
-    <row r="51" spans="1:6" s="18" customFormat="1" ht="75" customHeight="1">
+      <c r="D50" s="13"/>
+      <c r="E50" s="14"/>
+      <c r="F50" s="13"/>
+    </row>
+    <row r="51" spans="1:6" s="15" customFormat="1" ht="60" customHeight="1">
       <c r="A51" s="31" t="s">
         <v>91</v>
       </c>
       <c r="B51" s="34" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="C51" s="31" t="s">
-        <v>25</v>
+        <v>104</v>
       </c>
       <c r="D51" s="31" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="E51" s="31" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F51" s="31"/>
     </row>
-    <row r="52" spans="1:6" s="19" customFormat="1" ht="47.25">
+    <row r="52" spans="1:6" s="18" customFormat="1" ht="75" customHeight="1">
       <c r="A52" s="31" t="s">
         <v>91</v>
       </c>
       <c r="B52" s="34" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="C52" s="31" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="D52" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="E52" s="31"/>
+      <c r="E52" s="31" t="s">
+        <v>6</v>
+      </c>
       <c r="F52" s="31"/>
     </row>
-    <row r="53" spans="1:6" ht="60" customHeight="1">
+    <row r="53" spans="1:6" s="19" customFormat="1" ht="47.25">
       <c r="A53" s="31" t="s">
         <v>91</v>
       </c>
       <c r="B53" s="34" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C53" s="31" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="D53" s="31" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="E53" s="31"/>
       <c r="F53" s="31"/>
     </row>
-    <row r="54" spans="1:6" s="15" customFormat="1" ht="31.5">
+    <row r="54" spans="1:6" ht="60" customHeight="1">
       <c r="A54" s="31" t="s">
         <v>91</v>
       </c>
       <c r="B54" s="34" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="C54" s="31" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="D54" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="E54" s="34"/>
-      <c r="F54" s="31" t="s">
+      <c r="E54" s="31"/>
+      <c r="F54" s="31"/>
+    </row>
+    <row r="55" spans="1:6" s="15" customFormat="1" ht="31.5">
+      <c r="A55" s="31" t="s">
+        <v>91</v>
+      </c>
+      <c r="B55" s="34" t="s">
+        <v>69</v>
+      </c>
+      <c r="C55" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="D55" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="E55" s="34"/>
+      <c r="F55" s="31" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="55" spans="1:6" s="30" customFormat="1" ht="66" customHeight="1">
-      <c r="A55" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="B55" s="31" t="s">
-        <v>95</v>
-      </c>
-      <c r="C55" s="31" t="s">
-        <v>97</v>
-      </c>
-      <c r="D55" s="31" t="s">
-        <v>14</v>
-      </c>
-      <c r="E55" s="31"/>
-      <c r="F55" s="31"/>
     </row>
     <row r="56" spans="1:6" s="30" customFormat="1" ht="66" customHeight="1">
       <c r="A56" s="10" t="s">
         <v>91</v>
       </c>
       <c r="B56" s="31" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C56" s="31" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="D56" s="31" t="s">
         <v>14</v>
@@ -3702,33 +3712,31 @@
       <c r="E56" s="31"/>
       <c r="F56" s="31"/>
     </row>
-    <row r="57" spans="1:6" ht="83.25" customHeight="1">
-      <c r="A57" s="31" t="s">
+    <row r="57" spans="1:6" s="30" customFormat="1" ht="66" customHeight="1">
+      <c r="A57" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="B57" s="34" t="s">
-        <v>71</v>
+      <c r="B57" s="31" t="s">
+        <v>96</v>
       </c>
       <c r="C57" s="31" t="s">
-        <v>107</v>
+        <v>90</v>
       </c>
       <c r="D57" s="31" t="s">
-        <v>35</v>
-      </c>
-      <c r="E57" s="34" t="s">
-        <v>34</v>
-      </c>
-      <c r="F57" s="34"/>
-    </row>
-    <row r="58" spans="1:6" ht="78.75">
+        <v>14</v>
+      </c>
+      <c r="E57" s="31"/>
+      <c r="F57" s="31"/>
+    </row>
+    <row r="58" spans="1:6" ht="83.25" customHeight="1">
       <c r="A58" s="31" t="s">
         <v>91</v>
       </c>
       <c r="B58" s="34" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C58" s="31" t="s">
-        <v>36</v>
+        <v>105</v>
       </c>
       <c r="D58" s="31" t="s">
         <v>35</v>
@@ -3738,15 +3746,15 @@
       </c>
       <c r="F58" s="34"/>
     </row>
-    <row r="59" spans="1:6" ht="78.75" customHeight="1">
+    <row r="59" spans="1:6" ht="78.75">
       <c r="A59" s="31" t="s">
         <v>91</v>
       </c>
       <c r="B59" s="34" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C59" s="31" t="s">
-        <v>108</v>
+        <v>36</v>
       </c>
       <c r="D59" s="31" t="s">
         <v>35</v>
@@ -3756,75 +3764,77 @@
       </c>
       <c r="F59" s="34"/>
     </row>
-    <row r="60" spans="1:6" ht="72" customHeight="1">
+    <row r="60" spans="1:6" ht="78.75" customHeight="1">
       <c r="A60" s="31" t="s">
         <v>91</v>
       </c>
-      <c r="B60" s="31" t="s">
+      <c r="B60" s="34" t="s">
+        <v>73</v>
+      </c>
+      <c r="C60" s="31" t="s">
+        <v>106</v>
+      </c>
+      <c r="D60" s="31" t="s">
+        <v>35</v>
+      </c>
+      <c r="E60" s="34" t="s">
+        <v>34</v>
+      </c>
+      <c r="F60" s="34"/>
+    </row>
+    <row r="61" spans="1:6" ht="72" customHeight="1">
+      <c r="A61" s="31" t="s">
+        <v>91</v>
+      </c>
+      <c r="B61" s="31" t="s">
         <v>88</v>
       </c>
-      <c r="C60" s="31" t="s">
+      <c r="C61" s="31" t="s">
         <v>90</v>
       </c>
-      <c r="D60" s="31" t="s">
+      <c r="D61" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="E60" s="34"/>
-      <c r="F60" s="34"/>
-    </row>
-    <row r="61" spans="1:6" ht="60" customHeight="1">
-      <c r="A61" s="13" t="s">
+      <c r="E61" s="34"/>
+      <c r="F61" s="34"/>
+    </row>
+    <row r="62" spans="1:6" ht="60" customHeight="1">
+      <c r="A62" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="B61" s="13"/>
-      <c r="C61" s="13" t="s">
+      <c r="B62" s="13"/>
+      <c r="C62" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="D61" s="13"/>
-      <c r="E61" s="14"/>
-      <c r="F61" s="13"/>
-    </row>
-    <row r="62" spans="1:6" ht="60" customHeight="1">
-      <c r="A62" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="B62" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="C62" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D62" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E62" s="7"/>
-      <c r="F62" s="6"/>
+      <c r="D62" s="13"/>
+      <c r="E62" s="14"/>
+      <c r="F62" s="13"/>
     </row>
     <row r="63" spans="1:6" ht="60" customHeight="1">
       <c r="A63" s="6" t="s">
         <v>60</v>
       </c>
       <c r="B63" s="6" t="s">
-        <v>52</v>
+        <v>0</v>
       </c>
       <c r="C63" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D63" s="6" t="s">
         <v>14</v>
       </c>
       <c r="E63" s="7"/>
-      <c r="F63" s="7"/>
+      <c r="F63" s="6"/>
     </row>
     <row r="64" spans="1:6" ht="60" customHeight="1">
       <c r="A64" s="6" t="s">
         <v>60</v>
       </c>
       <c r="B64" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C64" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D64" s="6" t="s">
         <v>14</v>
@@ -3837,10 +3847,10 @@
         <v>60</v>
       </c>
       <c r="B65" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C65" s="6" t="s">
-        <v>33</v>
+        <v>13</v>
       </c>
       <c r="D65" s="6" t="s">
         <v>14</v>
@@ -3853,32 +3863,48 @@
         <v>60</v>
       </c>
       <c r="B66" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C66" s="6" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="D66" s="6" t="s">
         <v>14</v>
       </c>
       <c r="E66" s="7"/>
-      <c r="F66" s="6"/>
+      <c r="F66" s="7"/>
     </row>
     <row r="67" spans="1:6" ht="60" customHeight="1">
       <c r="A67" s="6" t="s">
         <v>60</v>
       </c>
       <c r="B67" s="6" t="s">
-        <v>1</v>
+        <v>55</v>
       </c>
       <c r="C67" s="6" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="D67" s="6" t="s">
         <v>14</v>
       </c>
       <c r="E67" s="7"/>
-      <c r="F67" s="7"/>
+      <c r="F67" s="6"/>
+    </row>
+    <row r="68" spans="1:6" ht="60" customHeight="1">
+      <c r="A68" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B68" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C68" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D68" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E68" s="7"/>
+      <c r="F68" s="7"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B4:B5 B9:B12">
@@ -3909,7 +3935,7 @@
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The format the field should follow" sqref="E1" xr:uid="{00000000-0002-0000-0600-000004000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The units the field should contain" sqref="F1" xr:uid="{00000000-0002-0000-0600-000005000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Latitude in decimal degrees to five decimal places" sqref="B18:B21" xr:uid="{00000000-0002-0000-0600-000006000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="A unique identifier used to identify a single taxon. Does not have to be a full scientific name, it can be a abbreviation or other, but in that case YOU MUST link that to scientific nomenclature in the 'TaxaList' sheet" sqref="B36:B37" xr:uid="{00000000-0002-0000-0600-000007000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="A unique identifier used to identify a single taxon. Does not have to be a full scientific name, it can be a abbreviation or other, but in that case YOU MUST link that to scientific nomenclature in the 'TaxaList' sheet" sqref="B37:B38" xr:uid="{00000000-0002-0000-0600-000007000000}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>